<commit_message>
Finished day eight, part 1.
</commit_message>
<xml_diff>
--- a/Day8/uppgift8.xlsx
+++ b/Day8/uppgift8.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/833e0ed7e335127c/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Src\AdventOfCode2022\Day8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{9BFC95A5-3F72-4772-BCDF-EF42D74811BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{580E330B-BBCE-4BDE-950A-A5702F69B15E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFDC722-6A67-4ECB-8346-266AF30BBA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E03B1014-F0C8-4A3A-A28D-C00BAC6F6474}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{E03B1014-F0C8-4A3A-A28D-C00BAC6F6474}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+  <si>
+    <t>Svep en rad I taget</t>
+  </si>
+  <si>
+    <t>Svep en kolumn I taget</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>3,0</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>4,0</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -46,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -56,6 +130,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -72,10 +158,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,22 +482,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AE625E-B82F-4499-8814-03E954209456}">
-  <dimension ref="A1:BK4"/>
+  <dimension ref="A1:BL26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BK1" sqref="BK1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="AM26" sqref="AM26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="62" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="38" width="1.7890625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="40" max="62" width="1.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="A1" s="1">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6">
         <v>5</v>
       </c>
       <c r="C1" s="1">
@@ -432,7 +526,7 @@
       <c r="J1" s="1">
         <v>1</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="6">
         <v>7</v>
       </c>
       <c r="L1" s="1">
@@ -462,7 +556,7 @@
       <c r="T1" s="1">
         <v>7</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U1" s="6">
         <v>8</v>
       </c>
       <c r="V1" s="1">
@@ -486,7 +580,7 @@
       <c r="AB1" s="1">
         <v>4</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC1" s="6">
         <v>9</v>
       </c>
       <c r="AD1" s="1">
@@ -567,7 +661,7 @@
       <c r="BC1" s="1">
         <v>6</v>
       </c>
-      <c r="BD1" s="1">
+      <c r="BD1" s="6">
         <v>9</v>
       </c>
       <c r="BE1" s="1">
@@ -576,7 +670,7 @@
       <c r="BF1" s="1">
         <v>5</v>
       </c>
-      <c r="BG1" s="1">
+      <c r="BG1" s="6">
         <v>7</v>
       </c>
       <c r="BH1" s="1">
@@ -585,19 +679,19 @@
       <c r="BI1" s="1">
         <v>5</v>
       </c>
-      <c r="BJ1" s="1">
+      <c r="BJ1" s="6">
         <v>5</v>
       </c>
       <c r="BK1">
-        <f>COUNT(A1:BJ4)-67</f>
+        <f>62*4-67</f>
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>6</v>
       </c>
       <c r="C2" s="1">
@@ -660,13 +754,13 @@
       <c r="V2">
         <v>3</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="6">
         <v>8</v>
       </c>
       <c r="X2">
         <v>2</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2" s="6">
         <v>9</v>
       </c>
       <c r="Z2">
@@ -765,7 +859,7 @@
       <c r="BE2" s="1">
         <v>6</v>
       </c>
-      <c r="BF2" s="1">
+      <c r="BF2" s="6">
         <v>9</v>
       </c>
       <c r="BG2" s="1">
@@ -777,15 +871,19 @@
       <c r="BI2">
         <v>5</v>
       </c>
-      <c r="BJ2" s="1">
-        <v>8</v>
+      <c r="BJ2" s="6">
+        <v>8</v>
+      </c>
+      <c r="BK2">
+        <f>62+28+29+62</f>
+        <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6">
         <v>6</v>
       </c>
       <c r="C3" s="1">
@@ -809,7 +907,7 @@
       <c r="I3" s="1">
         <v>6</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="6">
         <v>7</v>
       </c>
       <c r="K3">
@@ -851,7 +949,7 @@
       <c r="W3">
         <v>3</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="6">
         <v>8</v>
       </c>
       <c r="Y3">
@@ -866,7 +964,7 @@
       <c r="AB3">
         <v>8</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3" s="6">
         <v>9</v>
       </c>
       <c r="AD3">
@@ -935,7 +1033,7 @@
       <c r="AY3" s="1">
         <v>7</v>
       </c>
-      <c r="AZ3" s="1">
+      <c r="AZ3" s="6">
         <v>9</v>
       </c>
       <c r="BA3" s="1">
@@ -959,24 +1057,24 @@
       <c r="BG3" s="1">
         <v>8</v>
       </c>
-      <c r="BH3" s="1">
+      <c r="BH3" s="6">
         <v>8</v>
       </c>
       <c r="BI3" s="1">
         <v>6</v>
       </c>
-      <c r="BJ3" s="1">
+      <c r="BJ3" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>5</v>
       </c>
       <c r="D4" s="1">
@@ -1000,7 +1098,7 @@
       <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="6">
         <v>7</v>
       </c>
       <c r="L4" s="1">
@@ -1018,7 +1116,7 @@
       <c r="P4" s="1">
         <v>6</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="6">
         <v>8</v>
       </c>
       <c r="R4" s="1">
@@ -1057,7 +1155,7 @@
       <c r="AC4" s="1">
         <v>7</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AD4" s="6">
         <v>9</v>
       </c>
       <c r="AE4" s="1">
@@ -1117,7 +1215,7 @@
       <c r="AW4" s="1">
         <v>7</v>
       </c>
-      <c r="AX4" s="1">
+      <c r="AX4" s="6">
         <v>9</v>
       </c>
       <c r="AY4" s="1">
@@ -1135,7 +1233,7 @@
       <c r="BC4" s="1">
         <v>7</v>
       </c>
-      <c r="BD4" s="1">
+      <c r="BD4" s="6">
         <v>8</v>
       </c>
       <c r="BE4" s="1">
@@ -1150,11 +1248,1859 @@
       <c r="BH4" s="1">
         <v>7</v>
       </c>
-      <c r="BI4" s="1">
-        <v>7</v>
-      </c>
-      <c r="BJ4" s="1">
-        <v>5</v>
+      <c r="BI4" s="6">
+        <v>7</v>
+      </c>
+      <c r="BJ4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5">
+        <v>7</v>
+      </c>
+      <c r="L9" s="3">
+        <v>7</v>
+      </c>
+      <c r="M9" s="3">
+        <v>6</v>
+      </c>
+      <c r="N9" s="3">
+        <v>6</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>7</v>
+      </c>
+      <c r="R9" s="3">
+        <v>7</v>
+      </c>
+      <c r="S9" s="3">
+        <v>2</v>
+      </c>
+      <c r="T9" s="3">
+        <v>7</v>
+      </c>
+      <c r="U9" s="5">
+        <v>8</v>
+      </c>
+      <c r="V9" s="3">
+        <v>4</v>
+      </c>
+      <c r="W9" s="3">
+        <v>3</v>
+      </c>
+      <c r="X9" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>8</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>8</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>8</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>9</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>8</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>7</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>7</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>6</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>9</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>8</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>7</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>6</v>
+      </c>
+      <c r="BA9" s="3">
+        <v>7</v>
+      </c>
+      <c r="BB9" s="3">
+        <v>9</v>
+      </c>
+      <c r="BC9" s="3">
+        <v>6</v>
+      </c>
+      <c r="BD9" s="5">
+        <v>9</v>
+      </c>
+      <c r="BE9" s="3">
+        <v>5</v>
+      </c>
+      <c r="BF9" s="3">
+        <v>5</v>
+      </c>
+      <c r="BG9" s="5">
+        <v>7</v>
+      </c>
+      <c r="BH9" s="3">
+        <v>5</v>
+      </c>
+      <c r="BI9" s="3">
+        <v>5</v>
+      </c>
+      <c r="BJ9" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK9" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>5</v>
+      </c>
+      <c r="K10" s="5">
+        <v>7</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>5</v>
+      </c>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
+      <c r="O10" s="3">
+        <v>6</v>
+      </c>
+      <c r="P10" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>4</v>
+      </c>
+      <c r="R10" s="3">
+        <v>4</v>
+      </c>
+      <c r="S10" s="3">
+        <v>7</v>
+      </c>
+      <c r="T10" s="3">
+        <v>4</v>
+      </c>
+      <c r="U10" s="3">
+        <v>3</v>
+      </c>
+      <c r="V10" s="3">
+        <v>3</v>
+      </c>
+      <c r="W10" s="5">
+        <v>8</v>
+      </c>
+      <c r="X10" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>7</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>8</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>6</v>
+      </c>
+      <c r="AK10" s="3">
+        <v>9</v>
+      </c>
+      <c r="AL10" s="3">
+        <v>8</v>
+      </c>
+      <c r="AM10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>9</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>8</v>
+      </c>
+      <c r="AP10" s="3">
+        <v>8</v>
+      </c>
+      <c r="AQ10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AR10" s="3">
+        <v>6</v>
+      </c>
+      <c r="AS10" s="3">
+        <v>7</v>
+      </c>
+      <c r="AT10" s="3">
+        <v>6</v>
+      </c>
+      <c r="AU10" s="3">
+        <v>9</v>
+      </c>
+      <c r="AV10" s="3">
+        <v>7</v>
+      </c>
+      <c r="AW10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AX10" s="3">
+        <v>7</v>
+      </c>
+      <c r="AY10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AZ10" s="3">
+        <v>6</v>
+      </c>
+      <c r="BA10" s="3">
+        <v>5</v>
+      </c>
+      <c r="BB10" s="3">
+        <v>6</v>
+      </c>
+      <c r="BC10" s="3">
+        <v>9</v>
+      </c>
+      <c r="BD10" s="3">
+        <v>7</v>
+      </c>
+      <c r="BE10" s="3">
+        <v>6</v>
+      </c>
+      <c r="BF10" s="5">
+        <v>9</v>
+      </c>
+      <c r="BG10" s="3">
+        <v>8</v>
+      </c>
+      <c r="BH10" s="3">
+        <v>7</v>
+      </c>
+      <c r="BI10" s="3">
+        <v>5</v>
+      </c>
+      <c r="BJ10" s="5">
+        <v>8</v>
+      </c>
+      <c r="BK10" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5">
+        <v>7</v>
+      </c>
+      <c r="K11" s="3">
+        <v>3</v>
+      </c>
+      <c r="L11" s="3">
+        <v>3</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
+        <v>6</v>
+      </c>
+      <c r="O11" s="3">
+        <v>5</v>
+      </c>
+      <c r="P11" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>5</v>
+      </c>
+      <c r="R11" s="3">
+        <v>4</v>
+      </c>
+      <c r="S11" s="3">
+        <v>5</v>
+      </c>
+      <c r="T11" s="3">
+        <v>4</v>
+      </c>
+      <c r="U11" s="3">
+        <v>6</v>
+      </c>
+      <c r="V11" s="3">
+        <v>4</v>
+      </c>
+      <c r="W11" s="3">
+        <v>3</v>
+      </c>
+      <c r="X11" s="5">
+        <v>8</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>8</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>9</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>8</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>9</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>9</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>9</v>
+      </c>
+      <c r="AK11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AL11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AM11" s="3">
+        <v>9</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>4</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AP11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AR11" s="3">
+        <v>8</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>9</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV11" s="3">
+        <v>6</v>
+      </c>
+      <c r="AW11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AX11" s="3">
+        <v>5</v>
+      </c>
+      <c r="AY11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AZ11" s="5">
+        <v>9</v>
+      </c>
+      <c r="BA11" s="3">
+        <v>8</v>
+      </c>
+      <c r="BB11" s="3">
+        <v>5</v>
+      </c>
+      <c r="BC11" s="3">
+        <v>6</v>
+      </c>
+      <c r="BD11" s="3">
+        <v>8</v>
+      </c>
+      <c r="BE11" s="3">
+        <v>8</v>
+      </c>
+      <c r="BF11" s="3">
+        <v>8</v>
+      </c>
+      <c r="BG11" s="3">
+        <v>8</v>
+      </c>
+      <c r="BH11" s="5">
+        <v>8</v>
+      </c>
+      <c r="BI11" s="3">
+        <v>6</v>
+      </c>
+      <c r="BJ11" s="5">
+        <v>6</v>
+      </c>
+      <c r="BK11" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+      <c r="K12" s="5">
+        <v>7</v>
+      </c>
+      <c r="L12" s="3">
+        <v>7</v>
+      </c>
+      <c r="M12" s="3">
+        <v>5</v>
+      </c>
+      <c r="N12" s="3">
+        <v>4</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2</v>
+      </c>
+      <c r="P12" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>8</v>
+      </c>
+      <c r="R12" s="3">
+        <v>8</v>
+      </c>
+      <c r="S12" s="3">
+        <v>7</v>
+      </c>
+      <c r="T12" s="3">
+        <v>4</v>
+      </c>
+      <c r="U12" s="3">
+        <v>5</v>
+      </c>
+      <c r="V12" s="3">
+        <v>4</v>
+      </c>
+      <c r="W12" s="3">
+        <v>8</v>
+      </c>
+      <c r="X12" s="3">
+        <v>6</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>9</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>9</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>9</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AK12" s="3">
+        <v>8</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AP12" s="3">
+        <v>9</v>
+      </c>
+      <c r="AQ12" s="3">
+        <v>5</v>
+      </c>
+      <c r="AR12" s="3">
+        <v>9</v>
+      </c>
+      <c r="AS12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AT12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AV12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AW12" s="3">
+        <v>7</v>
+      </c>
+      <c r="AX12" s="5">
+        <v>9</v>
+      </c>
+      <c r="AY12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AZ12" s="3">
+        <v>8</v>
+      </c>
+      <c r="BA12" s="3">
+        <v>6</v>
+      </c>
+      <c r="BB12" s="3">
+        <v>5</v>
+      </c>
+      <c r="BC12" s="3">
+        <v>7</v>
+      </c>
+      <c r="BD12" s="5">
+        <v>8</v>
+      </c>
+      <c r="BE12" s="3">
+        <v>7</v>
+      </c>
+      <c r="BF12" s="3">
+        <v>5</v>
+      </c>
+      <c r="BG12" s="3">
+        <v>6</v>
+      </c>
+      <c r="BH12" s="3">
+        <v>7</v>
+      </c>
+      <c r="BI12" s="5">
+        <v>7</v>
+      </c>
+      <c r="BJ12" s="5">
+        <v>5</v>
+      </c>
+      <c r="BK12" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="BK13">
+        <f>SUM(BK9:BK12)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:63" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>5</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>7</v>
+      </c>
+      <c r="L16" s="1">
+        <v>7</v>
+      </c>
+      <c r="M16" s="1">
+        <v>6</v>
+      </c>
+      <c r="N16" s="1">
+        <v>6</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1</v>
+      </c>
+      <c r="P16" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>7</v>
+      </c>
+      <c r="R16" s="1">
+        <v>7</v>
+      </c>
+      <c r="S16" s="1">
+        <v>2</v>
+      </c>
+      <c r="T16" s="1">
+        <v>7</v>
+      </c>
+      <c r="U16" s="1">
+        <v>8</v>
+      </c>
+      <c r="V16" s="1">
+        <v>4</v>
+      </c>
+      <c r="W16" s="1">
+        <v>3</v>
+      </c>
+      <c r="X16" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>8</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE16" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AG16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>8</v>
+      </c>
+      <c r="AI16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AK16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AL16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>9</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AO16" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR16" s="1">
+        <v>8</v>
+      </c>
+      <c r="AS16" s="1">
+        <v>7</v>
+      </c>
+      <c r="AT16" s="1">
+        <v>7</v>
+      </c>
+      <c r="AU16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AV16" s="1">
+        <v>6</v>
+      </c>
+      <c r="AW16" s="1">
+        <v>9</v>
+      </c>
+      <c r="AX16" s="1">
+        <v>8</v>
+      </c>
+      <c r="AY16" s="1">
+        <v>7</v>
+      </c>
+      <c r="AZ16" s="1">
+        <v>6</v>
+      </c>
+      <c r="BA16" s="1">
+        <v>7</v>
+      </c>
+      <c r="BB16" s="1">
+        <v>9</v>
+      </c>
+      <c r="BC16" s="1">
+        <v>6</v>
+      </c>
+      <c r="BD16" s="1">
+        <v>9</v>
+      </c>
+      <c r="BE16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BF16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BG16" s="1">
+        <v>7</v>
+      </c>
+      <c r="BH16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI16" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3">
+        <v>4</v>
+      </c>
+      <c r="J17" s="1">
+        <v>5</v>
+      </c>
+      <c r="K17" s="3">
+        <v>7</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>5</v>
+      </c>
+      <c r="N17" s="3">
+        <v>2</v>
+      </c>
+      <c r="O17" s="1">
+        <v>6</v>
+      </c>
+      <c r="P17" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>4</v>
+      </c>
+      <c r="R17" s="3">
+        <v>4</v>
+      </c>
+      <c r="S17" s="1">
+        <v>7</v>
+      </c>
+      <c r="T17" s="3">
+        <v>4</v>
+      </c>
+      <c r="U17" s="3">
+        <v>3</v>
+      </c>
+      <c r="V17" s="3">
+        <v>3</v>
+      </c>
+      <c r="W17" s="1">
+        <v>8</v>
+      </c>
+      <c r="X17" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>9</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>4</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>7</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>5</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>5</v>
+      </c>
+      <c r="AI17" s="1">
+        <v>5</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>6</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>9</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>8</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>5</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>9</v>
+      </c>
+      <c r="AO17" s="1">
+        <v>8</v>
+      </c>
+      <c r="AP17" s="1">
+        <v>8</v>
+      </c>
+      <c r="AQ17" s="3">
+        <v>5</v>
+      </c>
+      <c r="AR17" s="3">
+        <v>6</v>
+      </c>
+      <c r="AS17" s="3">
+        <v>7</v>
+      </c>
+      <c r="AT17" s="3">
+        <v>6</v>
+      </c>
+      <c r="AU17" s="1">
+        <v>9</v>
+      </c>
+      <c r="AV17" s="1">
+        <v>7</v>
+      </c>
+      <c r="AW17" s="3">
+        <v>5</v>
+      </c>
+      <c r="AX17" s="3">
+        <v>7</v>
+      </c>
+      <c r="AY17" s="3">
+        <v>5</v>
+      </c>
+      <c r="AZ17" s="3">
+        <v>6</v>
+      </c>
+      <c r="BA17" s="3">
+        <v>5</v>
+      </c>
+      <c r="BB17" s="1">
+        <v>6</v>
+      </c>
+      <c r="BC17" s="1">
+        <v>9</v>
+      </c>
+      <c r="BD17" s="3">
+        <v>7</v>
+      </c>
+      <c r="BE17" s="1">
+        <v>6</v>
+      </c>
+      <c r="BF17" s="1">
+        <v>9</v>
+      </c>
+      <c r="BG17" s="1">
+        <v>8</v>
+      </c>
+      <c r="BH17" s="1">
+        <v>7</v>
+      </c>
+      <c r="BI17" s="3">
+        <v>5</v>
+      </c>
+      <c r="BJ17" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>6</v>
+      </c>
+      <c r="I18" s="1">
+        <v>6</v>
+      </c>
+      <c r="J18" s="1">
+        <v>7</v>
+      </c>
+      <c r="K18" s="3">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>6</v>
+      </c>
+      <c r="O18" s="1">
+        <v>5</v>
+      </c>
+      <c r="P18" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>5</v>
+      </c>
+      <c r="R18" s="3">
+        <v>4</v>
+      </c>
+      <c r="S18" s="3">
+        <v>5</v>
+      </c>
+      <c r="T18" s="3">
+        <v>4</v>
+      </c>
+      <c r="U18" s="1">
+        <v>6</v>
+      </c>
+      <c r="V18" s="3">
+        <v>4</v>
+      </c>
+      <c r="W18" s="3">
+        <v>3</v>
+      </c>
+      <c r="X18" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>8</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>8</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>9</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>4</v>
+      </c>
+      <c r="AE18" s="1">
+        <v>7</v>
+      </c>
+      <c r="AF18" s="1">
+        <v>8</v>
+      </c>
+      <c r="AG18" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>6</v>
+      </c>
+      <c r="AI18" s="1">
+        <v>9</v>
+      </c>
+      <c r="AJ18" s="1">
+        <v>9</v>
+      </c>
+      <c r="AK18" s="3">
+        <v>6</v>
+      </c>
+      <c r="AL18" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>9</v>
+      </c>
+      <c r="AN18" s="3">
+        <v>4</v>
+      </c>
+      <c r="AO18" s="3">
+        <v>5</v>
+      </c>
+      <c r="AP18" s="3">
+        <v>5</v>
+      </c>
+      <c r="AQ18" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR18" s="3">
+        <v>8</v>
+      </c>
+      <c r="AS18" s="1">
+        <v>9</v>
+      </c>
+      <c r="AT18" s="1">
+        <v>7</v>
+      </c>
+      <c r="AU18" s="3">
+        <v>6</v>
+      </c>
+      <c r="AV18" s="3">
+        <v>6</v>
+      </c>
+      <c r="AW18" s="3">
+        <v>7</v>
+      </c>
+      <c r="AX18" s="3">
+        <v>5</v>
+      </c>
+      <c r="AY18" s="1">
+        <v>7</v>
+      </c>
+      <c r="AZ18" s="1">
+        <v>9</v>
+      </c>
+      <c r="BA18" s="1">
+        <v>8</v>
+      </c>
+      <c r="BB18" s="3">
+        <v>5</v>
+      </c>
+      <c r="BC18" s="3">
+        <v>6</v>
+      </c>
+      <c r="BD18" s="3">
+        <v>8</v>
+      </c>
+      <c r="BE18" s="1">
+        <v>8</v>
+      </c>
+      <c r="BF18" s="1">
+        <v>8</v>
+      </c>
+      <c r="BG18" s="1">
+        <v>8</v>
+      </c>
+      <c r="BH18" s="1">
+        <v>8</v>
+      </c>
+      <c r="BI18" s="1">
+        <v>6</v>
+      </c>
+      <c r="BJ18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>5</v>
+      </c>
+      <c r="H19" s="1">
+        <v>5</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1">
+        <v>7</v>
+      </c>
+      <c r="L19" s="1">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1">
+        <v>5</v>
+      </c>
+      <c r="N19" s="1">
+        <v>4</v>
+      </c>
+      <c r="O19" s="1">
+        <v>2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>8</v>
+      </c>
+      <c r="R19" s="1">
+        <v>8</v>
+      </c>
+      <c r="S19" s="1">
+        <v>7</v>
+      </c>
+      <c r="T19" s="1">
+        <v>4</v>
+      </c>
+      <c r="U19" s="1">
+        <v>5</v>
+      </c>
+      <c r="V19" s="1">
+        <v>4</v>
+      </c>
+      <c r="W19" s="1">
+        <v>8</v>
+      </c>
+      <c r="X19" s="1">
+        <v>6</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>8</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AE19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AI19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AK19" s="1">
+        <v>8</v>
+      </c>
+      <c r="AL19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AN19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AO19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AQ19" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AU19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AV19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AW19" s="1">
+        <v>7</v>
+      </c>
+      <c r="AX19" s="1">
+        <v>9</v>
+      </c>
+      <c r="AY19" s="1">
+        <v>6</v>
+      </c>
+      <c r="AZ19" s="1">
+        <v>8</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>6</v>
+      </c>
+      <c r="BB19" s="1">
+        <v>5</v>
+      </c>
+      <c r="BC19" s="1">
+        <v>7</v>
+      </c>
+      <c r="BD19" s="1">
+        <v>8</v>
+      </c>
+      <c r="BE19" s="1">
+        <v>7</v>
+      </c>
+      <c r="BF19" s="1">
+        <v>5</v>
+      </c>
+      <c r="BG19" s="1">
+        <v>6</v>
+      </c>
+      <c r="BH19" s="1">
+        <v>7</v>
+      </c>
+      <c r="BI19" s="1">
+        <v>7</v>
+      </c>
+      <c r="BJ19" s="1">
+        <v>5</v>
+      </c>
+      <c r="BL19">
+        <f>62*4</f>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="E20" s="3">
+        <v>4</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3">
+        <v>4</v>
+      </c>
+      <c r="I20" s="3">
+        <v>3</v>
+      </c>
+      <c r="J20" s="3">
+        <v>4</v>
+      </c>
+      <c r="K20" s="3">
+        <v>2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <v>2</v>
+      </c>
+      <c r="N20" s="3">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3">
+        <v>4</v>
+      </c>
+      <c r="P20" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>2</v>
+      </c>
+      <c r="R20" s="3">
+        <v>2</v>
+      </c>
+      <c r="S20" s="3">
+        <v>3</v>
+      </c>
+      <c r="T20" s="3">
+        <v>2</v>
+      </c>
+      <c r="U20" s="3">
+        <v>3</v>
+      </c>
+      <c r="V20" s="3">
+        <v>2</v>
+      </c>
+      <c r="W20" s="3">
+        <v>3</v>
+      </c>
+      <c r="X20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>4</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AJ20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AK20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AL20" s="3">
+        <v>4</v>
+      </c>
+      <c r="AM20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AO20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AP20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AQ20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AR20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AS20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AT20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AU20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AV20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AW20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AX20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AY20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AZ20" s="3">
+        <v>3</v>
+      </c>
+      <c r="BA20" s="3">
+        <v>3</v>
+      </c>
+      <c r="BB20" s="3">
+        <v>3</v>
+      </c>
+      <c r="BC20" s="3">
+        <v>3</v>
+      </c>
+      <c r="BD20" s="3">
+        <v>2</v>
+      </c>
+      <c r="BE20" s="3">
+        <v>4</v>
+      </c>
+      <c r="BF20" s="3">
+        <v>4</v>
+      </c>
+      <c r="BG20" s="3">
+        <v>4</v>
+      </c>
+      <c r="BH20" s="3">
+        <v>4</v>
+      </c>
+      <c r="BI20" s="3">
+        <v>3</v>
+      </c>
+      <c r="BJ20" s="3">
+        <v>4</v>
+      </c>
+      <c r="BK20">
+        <f>SUM(A20:BJ20)</f>
+        <v>190</v>
+      </c>
+      <c r="BL20">
+        <f>62*4-58</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:64" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q26" s="7"/>
+      <c r="S26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM26">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>